<commit_message>
Added some alternative components
</commit_message>
<xml_diff>
--- a/BOM_v04_2.xlsx
+++ b/BOM_v04_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="9" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1270" uniqueCount="480">
   <si>
     <t>Value</t>
   </si>
@@ -1506,6 +1506,18 @@
   </si>
   <si>
     <t>ADM7151ARDZ-04-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">873-SKY13343-92LF </t>
+  </si>
+  <si>
+    <t>LP3876ESXADJNOPB</t>
+  </si>
+  <si>
+    <t>Alternatives</t>
+  </si>
+  <si>
+    <t>ADM7151_ARDZ-07-R7 (slight PCB mod required)</t>
   </si>
 </sst>
 </file>
@@ -1852,7 +1864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+    <sheetView topLeftCell="A181" workbookViewId="0">
       <selection activeCell="B208" sqref="B208"/>
     </sheetView>
   </sheetViews>
@@ -5996,10 +6008,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F72"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6009,9 +6021,10 @@
     <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.7109375" customWidth="1"/>
     <col min="5" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="41.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>124</v>
       </c>
@@ -6021,8 +6034,11 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>7</v>
       </c>
@@ -6033,7 +6049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>7</v>
       </c>
@@ -6044,7 +6060,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>2</v>
       </c>
@@ -6055,7 +6071,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>3</v>
       </c>
@@ -6066,7 +6082,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>9</v>
       </c>
@@ -6077,7 +6093,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>4</v>
       </c>
@@ -6088,7 +6104,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>17</v>
       </c>
@@ -6109,7 +6125,7 @@
         <v>2.5499999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>7</v>
       </c>
@@ -6120,7 +6136,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>2</v>
       </c>
@@ -6131,7 +6147,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>6</v>
       </c>
@@ -6145,7 +6161,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>10</v>
       </c>
@@ -6159,7 +6175,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>2</v>
       </c>
@@ -6170,7 +6186,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>2</v>
       </c>
@@ -6181,7 +6197,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>2</v>
       </c>
@@ -6192,7 +6208,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>63</v>
       </c>
@@ -6639,7 +6655,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:7">
       <c r="A49">
         <v>1</v>
       </c>
@@ -6650,7 +6666,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:7">
       <c r="A50">
         <v>2</v>
       </c>
@@ -6661,7 +6677,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:7">
       <c r="A51">
         <v>1</v>
       </c>
@@ -6672,7 +6688,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:7">
       <c r="A52">
         <v>2</v>
       </c>
@@ -6683,7 +6699,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:7">
       <c r="A53">
         <v>2</v>
       </c>
@@ -6694,7 +6710,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:7">
       <c r="A54">
         <v>1</v>
       </c>
@@ -6705,7 +6721,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:7">
       <c r="A55">
         <v>2</v>
       </c>
@@ -6716,7 +6732,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:7">
       <c r="A56">
         <v>2</v>
       </c>
@@ -6727,7 +6743,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:7">
       <c r="A57">
         <v>1</v>
       </c>
@@ -6738,7 +6754,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:7">
       <c r="A58">
         <v>23</v>
       </c>
@@ -6749,11 +6765,11 @@
         <v>0.05</v>
       </c>
       <c r="F58">
-        <f>A58*E58</f>
+        <f t="shared" ref="F58:F70" si="0">A58*E58</f>
         <v>1.1500000000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:7">
       <c r="A59">
         <v>2</v>
       </c>
@@ -6770,11 +6786,11 @@
         <v>2.71</v>
       </c>
       <c r="F59">
-        <f>A59*E59</f>
+        <f t="shared" si="0"/>
         <v>5.42</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:7">
       <c r="A60">
         <v>1</v>
       </c>
@@ -6791,11 +6807,11 @@
         <v>14.99</v>
       </c>
       <c r="F60">
-        <f>A60*E60</f>
+        <f t="shared" si="0"/>
         <v>14.99</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:7">
       <c r="A61">
         <v>1</v>
       </c>
@@ -6812,11 +6828,11 @@
         <v>0.26</v>
       </c>
       <c r="F61">
-        <f>A61*E61</f>
+        <f t="shared" si="0"/>
         <v>0.26</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:7">
       <c r="A62">
         <v>2</v>
       </c>
@@ -6833,11 +6849,14 @@
         <v>1.44</v>
       </c>
       <c r="F62">
-        <f>A62*E62</f>
+        <f t="shared" si="0"/>
         <v>2.88</v>
       </c>
-    </row>
-    <row r="63" spans="1:6">
+      <c r="G62" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63">
         <v>1</v>
       </c>
@@ -6854,11 +6873,11 @@
         <v>3.21</v>
       </c>
       <c r="F63">
-        <f>A63*E63</f>
+        <f t="shared" si="0"/>
         <v>3.21</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:7">
       <c r="A64">
         <v>1</v>
       </c>
@@ -6875,11 +6894,11 @@
         <v>4.0599999999999996</v>
       </c>
       <c r="F64">
-        <f>A64*E64</f>
+        <f t="shared" si="0"/>
         <v>4.0599999999999996</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:7">
       <c r="A65">
         <v>2</v>
       </c>
@@ -6896,11 +6915,14 @@
         <v>2.11</v>
       </c>
       <c r="F65">
-        <f>A65*E65</f>
+        <f t="shared" si="0"/>
         <v>4.22</v>
       </c>
-    </row>
-    <row r="66" spans="1:6">
+      <c r="G65" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66">
         <v>2</v>
       </c>
@@ -6917,11 +6939,11 @@
         <v>0.86</v>
       </c>
       <c r="F66">
-        <f>A66*E66</f>
+        <f t="shared" si="0"/>
         <v>1.72</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:7">
       <c r="A67">
         <v>1</v>
       </c>
@@ -6938,11 +6960,11 @@
         <v>0.95</v>
       </c>
       <c r="F67">
-        <f>A67*E67</f>
+        <f t="shared" si="0"/>
         <v>0.95</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:7">
       <c r="A68">
         <v>1</v>
       </c>
@@ -6959,11 +6981,11 @@
         <v>1.18</v>
       </c>
       <c r="F68">
-        <f>A68*E68</f>
+        <f t="shared" si="0"/>
         <v>1.18</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:7">
       <c r="A69">
         <v>1</v>
       </c>
@@ -6980,11 +7002,14 @@
         <v>8.0399999999999991</v>
       </c>
       <c r="F69">
-        <f>A69*E69</f>
+        <f t="shared" si="0"/>
         <v>8.0399999999999991</v>
       </c>
-    </row>
-    <row r="70" spans="1:6">
+      <c r="G69" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70">
         <v>2</v>
       </c>
@@ -7001,11 +7026,11 @@
         <v>16.78</v>
       </c>
       <c r="F70">
-        <f>A70*E70</f>
+        <f t="shared" si="0"/>
         <v>33.56</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:7">
       <c r="F72">
         <f>SUM(F2:F71)</f>
         <v>96.09</v>

</xml_diff>